<commit_message>
Fixed bug in path recognition
</commit_message>
<xml_diff>
--- a/excell/28.xlsx
+++ b/excell/28.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+  <si>
+    <t>6E</t>
+  </si>
+  <si>
+    <t>7E</t>
+  </si>
   <si>
     <t>8E</t>
   </si>
@@ -28,53 +34,75 @@
     <t>11E</t>
   </si>
   <si>
-    <t>6E</t>
-  </si>
-  <si>
-    <t>7E</t>
+    <t>Среда
+15 Фев.</t>
+  </si>
+  <si>
+    <t>История (Настя)</t>
+  </si>
+  <si>
+    <t>Физ-ра (ЖК)</t>
+  </si>
+  <si>
+    <t>Четверг
+16 Фев.</t>
+  </si>
+  <si>
+    <t>География (ГН)</t>
+  </si>
+  <si>
+    <t>Физика (ЮН)</t>
+  </si>
+  <si>
+    <t>Информатика (Ок)</t>
   </si>
   <si>
     <t>Пяница
-20 Янв.</t>
-  </si>
-  <si>
-    <t>Химия (Greeeg)</t>
-  </si>
-  <si>
-    <t>Химия (G1234re213)</t>
-  </si>
-  <si>
-    <t>Физика (ЮН)</t>
-  </si>
-  <si>
-    <t>Англ.яз. (Ольга)</t>
+17 Фев.</t>
   </si>
   <si>
     <t>Суббота
-21 Янв.</t>
-  </si>
-  <si>
-    <t>География (Гриц)</t>
+18 Фев.</t>
   </si>
   <si>
     <t>Понедельн.
-22 Янв.</t>
+19 Фев.</t>
   </si>
   <si>
     <t>Понедельн.
-23 Янв.</t>
+20 Фев.</t>
   </si>
   <si>
     <t>Вторник
-24 Янв.</t>
+21 Фев.</t>
   </si>
   <si>
     <t>Среда
-25 Янв.</t>
+22 Фев.</t>
   </si>
   <si>
     <t>Четверг
-26 Янв.</t>
+23 Фев.</t>
+  </si>
+  <si>
+    <t>Пяница
+24 Фев.</t>
+  </si>
+  <si>
+    <t>Суббота
+25 Фев.</t>
+  </si>
+  <si>
+    <t>Понедельн.
+26 Фев.</t>
+  </si>
+  <si>
+    <t>Понедельн.
+27 Фев.</t>
+  </si>
+  <si>
+    <t>Вторник
+28 Фев.</t>
   </si>
 </sst>
 </file>
@@ -95,7 +123,7 @@
       <color rgb="00000000"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -104,13 +132,33 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFF01"/>
+        <fgColor rgb="00bb7bee"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00c48200"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="009E9E9E"/>
         <bgColor rgb="009E9E9E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="006a8200"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00af8500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00dc8300"/>
       </patternFill>
     </fill>
   </fills>
@@ -126,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -138,7 +186,19 @@
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -436,7 +496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,74 +534,65 @@
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="23" r="2" spans="1:8">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:8">
+      <c r="B3" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="4" spans="1:8">
+      <c r="B4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="3" spans="1:8">
-      <c r="B3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="5" spans="1:8">
+      <c r="B5" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="6" spans="1:8">
+      <c r="B6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row customHeight="1" ht="23" r="4" spans="1:8">
-      <c r="B4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4" t="s">
+    <row r="7" spans="1:8">
+      <c r="A7" s="6" t="n"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="27" r="5" spans="1:8">
-      <c r="B5" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="B8" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="23" r="9" spans="1:8">
+      <c r="B9" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="B6" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="5" t="n"/>
-    </row>
-    <row customHeight="1" ht="27" r="8" spans="1:8">
-      <c r="A8" s="2" t="s">
+    <row customHeight="1" ht="18" r="10" spans="1:8">
+      <c r="B10" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="B9" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="27" r="10" spans="1:8">
-      <c r="B10" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -549,16 +600,16 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="12" spans="1:8">
+    <row customHeight="1" ht="27" r="12" spans="1:8">
       <c r="B12" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>9</v>
+      <c r="C12" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="5" t="n"/>
+      <c r="A13" s="6" t="n"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
@@ -568,15 +619,9 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="15" spans="1:8">
+    <row r="15" spans="1:8">
       <c r="B15" s="3" t="n">
         <v>2</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -595,7 +640,7 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="5" t="n"/>
+      <c r="A19" s="6" t="n"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
@@ -626,7 +671,7 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="5" t="n"/>
+      <c r="A25" s="6" t="n"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
@@ -657,7 +702,7 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="5" t="n"/>
+      <c r="A31" s="6" t="n"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
@@ -688,7 +733,7 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="5" t="n"/>
+      <c r="A37" s="6" t="n"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="2" t="s">
@@ -718,8 +763,225 @@
         <v>5</v>
       </c>
     </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="6" t="n"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="B45" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="B46" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="B47" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="B48" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="6" t="n"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="B51" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="B52" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="B53" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="B54" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="6" t="n"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="B57" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="B58" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="B59" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="B60" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="6" t="n"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B62" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="B63" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="B64" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="B65" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="B66" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="6" t="n"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="B69" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="B70" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="B71" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="B72" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="6" t="n"/>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B74" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="B75" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="B76" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="B77" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="B78" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="6" t="n"/>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="B81" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="B82" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="B83" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="B84" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="27">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A7:H7"/>
@@ -733,6 +995,20 @@
     <mergeCell ref="A31:H31"/>
     <mergeCell ref="A38:A42"/>
     <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A43:H43"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A49:H49"/>
+    <mergeCell ref="A56:A60"/>
+    <mergeCell ref="A55:H55"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="A61:H61"/>
+    <mergeCell ref="A68:A72"/>
+    <mergeCell ref="A67:H67"/>
+    <mergeCell ref="A74:A78"/>
+    <mergeCell ref="A73:H73"/>
+    <mergeCell ref="A80:A84"/>
+    <mergeCell ref="A79:H79"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed some stuff =), added scroll to the class-listy
</commit_message>
<xml_diff>
--- a/excell/28.xlsx
+++ b/excell/28.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>6E</t>
   </si>
@@ -41,6 +41,12 @@
     <t>История (Настя)</t>
   </si>
   <si>
+    <t>Алгебра (Володя)</t>
+  </si>
+  <si>
+    <t>Физика (Ваня)</t>
+  </si>
+  <si>
     <t>Физ-ра (ЖК)</t>
   </si>
   <si>
@@ -48,6 +54,9 @@
 16 Фев.</t>
   </si>
   <si>
+    <t>Англ.яз. (Марина)</t>
+  </si>
+  <si>
     <t>География (ГН)</t>
   </si>
   <si>
@@ -64,6 +73,12 @@
 17 Фев.</t>
   </si>
   <si>
+    <t>Руск. яз (Маша К)</t>
+  </si>
+  <si>
+    <t>Литература (Алиса)</t>
+  </si>
+  <si>
     <t>Суббота
 18 Фев.</t>
   </si>
@@ -72,16 +87,25 @@
 19 Фев.</t>
   </si>
   <si>
+    <t>История (Катя)</t>
+  </si>
+  <si>
     <t>Понедельн.
 20 Фев.</t>
   </si>
   <si>
+    <t>Биология (Таня)</t>
+  </si>
+  <si>
     <t>Вторник
 21 Фев.</t>
   </si>
   <si>
     <t>Среда
 22 Фев.</t>
+  </si>
+  <si>
+    <t>Сл-сть (Маша С)</t>
   </si>
   <si>
     <t>Четверг
@@ -126,7 +150,7 @@
       <color rgb="00000000"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="17">
     <fill>
       <patternFill/>
     </fill>
@@ -136,6 +160,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00bb7bee"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00aa2dde"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0090eae9"/>
       </patternFill>
     </fill>
     <fill>
@@ -151,6 +185,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="001f8b2b"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="006a8200"/>
       </patternFill>
     </fill>
@@ -167,6 +206,31 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="003df85a"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0076902e"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="003c283c"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00238eed"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="008030f1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="007d902e"/>
       </patternFill>
     </fill>
   </fills>
@@ -182,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -197,17 +261,41 @@
     <xf applyAlignment="1" borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf borderId="0" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="8" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="9" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="10" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="11" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="12" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="13" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="14" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="15" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="16" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -558,89 +646,122 @@
         <v>2</v>
       </c>
     </row>
-    <row customHeight="1" ht="25" r="4" spans="1:8">
+    <row customHeight="1" ht="27" r="4" spans="1:8">
       <c r="B4" s="3" t="n">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="22" r="5" spans="1:8">
       <c r="B5" s="3" t="n">
         <v>4</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="6" spans="1:8">
       <c r="B6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>8</v>
+      <c r="C6" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="6" t="n"/>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="A7" s="8" t="n"/>
+    </row>
+    <row customHeight="1" ht="29" r="8" spans="1:8">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>1</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row customHeight="1" ht="23" r="9" spans="1:8">
       <c r="B9" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>10</v>
+      <c r="C9" s="10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="10" spans="1:8">
       <c r="B10" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="C10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="11" spans="1:8">
       <c r="B11" s="3" t="n">
         <v>4</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row customHeight="1" ht="69" r="12" spans="1:8">
       <c r="B12" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>13</v>
+      <c r="C12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="6" t="n"/>
+      <c r="A13" s="8" t="n"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B14" s="3" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row customHeight="1" ht="23" r="15" spans="1:8">
       <c r="B15" s="3" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="E15" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="29" r="16" spans="1:8">
       <c r="B16" s="3" t="n">
         <v>3</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -648,23 +769,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row customHeight="1" ht="30" r="18" spans="1:8">
       <c r="B18" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="C18" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="6" t="n"/>
+      <c r="A19" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="69" r="20" spans="1:8">
       <c r="A20" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B20" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H20" s="10" t="s">
-        <v>13</v>
+      <c r="H20" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -672,9 +799,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row customHeight="1" ht="27" r="22" spans="1:8">
       <c r="B22" s="3" t="n">
         <v>3</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -688,11 +818,11 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="6" t="n"/>
+      <c r="A25" s="8" t="n"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B26" s="3" t="n">
         <v>1</v>
@@ -703,9 +833,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row customHeight="1" ht="18" r="28" spans="1:8">
       <c r="B28" s="3" t="n">
         <v>3</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -713,17 +846,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row customHeight="1" ht="23" r="30" spans="1:8">
       <c r="B30" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="H30" s="16" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="6" t="n"/>
+      <c r="A31" s="8" t="n"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B32" s="3" t="n">
         <v>1</v>
@@ -744,17 +880,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row customHeight="1" ht="25" r="36" spans="1:8">
       <c r="B36" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="H36" s="17" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="6" t="n"/>
+      <c r="A37" s="8" t="n"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B38" s="3" t="n">
         <v>1</v>
@@ -781,11 +920,11 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="6" t="n"/>
+      <c r="A43" s="8" t="n"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B44" s="3" t="n">
         <v>1</v>
@@ -796,27 +935,39 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row customHeight="1" ht="25" r="46" spans="1:8">
       <c r="B46" s="3" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="C46" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="47" spans="1:8">
       <c r="B47" s="3" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="G47" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="25" r="48" spans="1:8">
       <c r="B48" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="C48" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="6" t="n"/>
+      <c r="A49" s="8" t="n"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B50" s="3" t="n">
         <v>1</v>
@@ -843,11 +994,11 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="6" t="n"/>
+      <c r="A55" s="8" t="n"/>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B56" s="3" t="n">
         <v>1</v>
@@ -874,11 +1025,11 @@
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="6" t="n"/>
+      <c r="A61" s="8" t="n"/>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B62" s="3" t="n">
         <v>1</v>
@@ -905,11 +1056,11 @@
       </c>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="6" t="n"/>
+      <c r="A67" s="8" t="n"/>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B68" s="3" t="n">
         <v>1</v>
@@ -936,11 +1087,11 @@
       </c>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="6" t="n"/>
+      <c r="A73" s="8" t="n"/>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B74" s="3" t="n">
         <v>1</v>
@@ -967,11 +1118,11 @@
       </c>
     </row>
     <row r="79" spans="1:8">
-      <c r="A79" s="6" t="n"/>
+      <c r="A79" s="8" t="n"/>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B80" s="3" t="n">
         <v>1</v>

</xml_diff>